<commit_message>
2014 Metadata links updated
</commit_message>
<xml_diff>
--- a/static/download/2014/RP1_APT_ASMA_2014.xlsx
+++ b/static/download/2014/RP1_APT_ASMA_2014.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ASMA_APT" sheetId="1" r:id="rId3"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -43,7 +43,7 @@
     <t>Meta data</t>
   </si>
   <si>
-    <t>ASMA additional time</t>
+    <t>Metadata - Single European Sky Portal</t>
   </si>
   <si>
     <t>Release date</t>
@@ -55,7 +55,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>NSA-PRU-Support@eurocontrol.int</t>
+    <t>pru-support@eurocontrol.int</t>
   </si>
   <si>
     <t>JAN-DEC</t>
@@ -589,8 +589,8 @@
     <font>
       <u/>
       <sz val="9.0"/>
-      <color rgb="FF396EA2"/>
-      <name val="Calibri"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -650,7 +650,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
+    <border/>
     <border>
       <left/>
       <right/>
@@ -771,204 +772,220 @@
   </cellStyleXfs>
   <cellXfs count="72">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="4" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="4" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="17" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -978,37 +995,40 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="19.71"/>
-    <col customWidth="1" min="4" max="4" width="13.86"/>
-    <col customWidth="1" min="5" max="5" width="10.14"/>
-    <col customWidth="1" min="6" max="7" width="11.57"/>
-    <col customWidth="1" min="8" max="8" width="11.0"/>
-    <col customWidth="1" min="9" max="9" width="22.57"/>
+    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" min="3" max="3" width="17.25"/>
+    <col customWidth="1" min="4" max="4" width="12.13"/>
+    <col customWidth="1" min="5" max="5" width="8.88"/>
+    <col customWidth="1" min="6" max="7" width="10.13"/>
+    <col customWidth="1" min="8" max="8" width="9.63"/>
+    <col customWidth="1" min="9" max="9" width="19.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2169,18 +2189,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.86"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="10.43"/>
-    <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="5" max="5" width="9.0"/>
-    <col customWidth="1" min="6" max="6" width="30.43"/>
+    <col customWidth="1" min="1" max="1" width="12.13"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" min="3" max="3" width="9.13"/>
+    <col customWidth="1" min="4" max="4" width="19.13"/>
+    <col customWidth="1" min="5" max="5" width="7.88"/>
+    <col customWidth="1" min="6" max="6" width="26.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2322,19 +2345,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.86"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="10.43"/>
-    <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="5" max="5" width="12.71"/>
-    <col customWidth="1" min="6" max="6" width="26.0"/>
-    <col customWidth="1" min="7" max="7" width="22.86"/>
+    <col customWidth="1" min="1" max="1" width="11.25"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" min="3" max="3" width="9.13"/>
+    <col customWidth="1" min="4" max="4" width="19.13"/>
+    <col customWidth="1" min="5" max="5" width="11.13"/>
+    <col customWidth="1" min="6" max="6" width="22.75"/>
+    <col customWidth="1" min="7" max="7" width="20.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -3387,23 +3413,25 @@
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F1"/>
-    <hyperlink r:id="rId2" ref="F2"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.57"/>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="8.0"/>
-    <col customWidth="1" min="4" max="4" width="113.57"/>
+    <col customWidth="1" min="1" max="1" width="9.25"/>
+    <col customWidth="1" min="2" max="2" width="15.88"/>
+    <col customWidth="1" min="3" max="3" width="7.0"/>
+    <col customWidth="1" min="4" max="4" width="99.38"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">

</xml_diff>